<commit_message>
update item template: add notes to give hints about each field
</commit_message>
<xml_diff>
--- a/frontend/public/con2-item-template.xlsx
+++ b/frontend/public/con2-item-template.xlsx
@@ -8,6 +8,64 @@
   <definedNames/>
   <calcPr/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A1">
+      <text>
+        <t xml:space="preserve">Item Name (english)
+Optional, but we do require name, type and description for at least one language (finnish or english)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B1">
+      <text>
+        <t xml:space="preserve">Item Type (english)
+Optional, but we do require name, type and description for at least one language (finnish or english)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C1">
+      <text>
+        <t xml:space="preserve">Item Description (english)
+Optional, but we do require name, type and description for at least one language (finnish or english)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D1">
+      <text>
+        <t xml:space="preserve">Item Name (finnish)
+Optional, but we do require name, type and description for at least one language (finnish or english)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E1">
+      <text>
+        <t xml:space="preserve">Item Type (finnish)
+Optional, but we do require name, type and description for at least one language (finnish or english)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F1">
+      <text>
+        <t xml:space="preserve">Item Description (finnish)
+Optional, but we do require name, type and description for at least one language (finnish or english)</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="G1">
+      <text>
+        <t xml:space="preserve">Quantity.
+Required. Total amount of the item</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="H1">
+      <text>
+        <t xml:space="preserve">Tags.
+Optional, but these help users find your item when searching on the site, and we do encourage their usage</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -315,8 +373,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.5"/>
-    <col customWidth="1" min="2" max="2" width="19.88"/>
+    <col customWidth="1" min="1" max="2" width="19.88"/>
     <col customWidth="1" min="3" max="3" width="25.75"/>
     <col customWidth="1" min="4" max="4" width="20.63"/>
     <col customWidth="1" min="5" max="5" width="17.38"/>
@@ -456,6 +513,7 @@
       <c r="H12" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>